<commit_message>
1, finished preliminary database
</commit_message>
<xml_diff>
--- a/data/map pasadena data set.xlsx
+++ b/data/map pasadena data set.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3318" uniqueCount="2141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3502" uniqueCount="2141">
   <si>
     <t>COMPLETE</t>
   </si>
@@ -6999,9 +6999,9 @@
   <dimension ref="A1:L406"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A199" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A366" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A207" activeCellId="0" sqref="A207:A217"/>
+      <selection pane="bottomLeft" activeCell="A367" activeCellId="0" sqref="A367:A386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.65"/>
@@ -10572,7 +10572,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="147" s="33" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
         <v>45</v>
       </c>
@@ -12067,6 +12067,9 @@
       </c>
     </row>
     <row r="218" s="16" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A218" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B218" s="16" t="s">
         <v>1000</v>
       </c>
@@ -12074,6 +12077,9 @@
       <c r="H218" s="31"/>
     </row>
     <row r="219" s="21" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A219" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B219" s="21" t="s">
         <v>1001</v>
       </c>
@@ -12095,6 +12101,9 @@
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A220" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B220" s="0" t="s">
         <v>1005</v>
       </c>
@@ -12112,6 +12121,9 @@
       </c>
     </row>
     <row r="221" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A221" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B221" s="0" t="s">
         <v>1008</v>
       </c>
@@ -12129,6 +12141,9 @@
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A222" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B222" s="0" t="s">
         <v>1012</v>
       </c>
@@ -12146,6 +12161,9 @@
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A223" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B223" s="0" t="s">
         <v>1016</v>
       </c>
@@ -12163,6 +12181,9 @@
       </c>
     </row>
     <row r="224" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A224" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B224" s="0" t="s">
         <v>101</v>
       </c>
@@ -12180,6 +12201,9 @@
       </c>
     </row>
     <row r="225" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A225" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B225" s="0" t="s">
         <v>1023</v>
       </c>
@@ -12197,6 +12221,9 @@
       </c>
     </row>
     <row r="226" s="7" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A226" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B226" s="7" t="s">
         <v>1027</v>
       </c>
@@ -12215,6 +12242,9 @@
       <c r="H226" s="8"/>
     </row>
     <row r="227" s="24" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A227" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B227" s="24" t="s">
         <v>1031</v>
       </c>
@@ -12233,6 +12263,9 @@
       <c r="H227" s="25"/>
     </row>
     <row r="228" s="24" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A228" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B228" s="24" t="s">
         <v>1035</v>
       </c>
@@ -12251,6 +12284,9 @@
       <c r="H228" s="25"/>
     </row>
     <row r="229" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A229" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B229" s="0" t="s">
         <v>1039</v>
       </c>
@@ -12268,6 +12304,9 @@
       </c>
     </row>
     <row r="230" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A230" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B230" s="0" t="s">
         <v>1042</v>
       </c>
@@ -12285,6 +12324,9 @@
       </c>
     </row>
     <row r="231" s="16" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A231" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B231" s="16" t="s">
         <v>1045</v>
       </c>
@@ -12292,6 +12334,9 @@
       <c r="H231" s="31"/>
     </row>
     <row r="232" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A232" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B232" s="0" t="s">
         <v>1046</v>
       </c>
@@ -12309,6 +12354,9 @@
       </c>
     </row>
     <row r="233" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A233" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B233" s="0" t="s">
         <v>1050</v>
       </c>
@@ -12329,6 +12377,9 @@
       </c>
     </row>
     <row r="234" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A234" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B234" s="0" t="s">
         <v>824</v>
       </c>
@@ -12349,6 +12400,9 @@
       </c>
     </row>
     <row r="235" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A235" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B235" s="0" t="s">
         <v>1059</v>
       </c>
@@ -12366,6 +12420,9 @@
       </c>
     </row>
     <row r="236" s="33" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A236" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B236" s="33" t="s">
         <v>1062</v>
       </c>
@@ -12387,6 +12444,9 @@
       </c>
     </row>
     <row r="237" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A237" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B237" s="0" t="s">
         <v>479</v>
       </c>
@@ -12407,6 +12467,9 @@
       </c>
     </row>
     <row r="238" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A238" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B238" s="0" t="s">
         <v>1071</v>
       </c>
@@ -12427,6 +12490,9 @@
       </c>
     </row>
     <row r="239" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A239" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B239" s="0" t="s">
         <v>1075</v>
       </c>
@@ -12444,6 +12510,9 @@
       </c>
     </row>
     <row r="240" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A240" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B240" s="0" t="s">
         <v>1079</v>
       </c>
@@ -12461,6 +12530,9 @@
       </c>
     </row>
     <row r="241" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A241" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B241" s="0" t="s">
         <v>1082</v>
       </c>
@@ -12481,6 +12553,9 @@
       </c>
     </row>
     <row r="242" s="28" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A242" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B242" s="28" t="s">
         <v>1087</v>
       </c>
@@ -12505,6 +12580,9 @@
       </c>
     </row>
     <row r="243" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A243" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B243" s="0" t="s">
         <v>1093</v>
       </c>
@@ -12528,6 +12606,9 @@
       </c>
     </row>
     <row r="244" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A244" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B244" s="0" t="s">
         <v>1097</v>
       </c>
@@ -12551,6 +12632,9 @@
       </c>
     </row>
     <row r="245" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A245" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B245" s="0" t="s">
         <v>1100</v>
       </c>
@@ -12571,6 +12655,9 @@
       </c>
     </row>
     <row r="246" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A246" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B246" s="0" t="s">
         <v>1105</v>
       </c>
@@ -12591,6 +12678,9 @@
       </c>
     </row>
     <row r="247" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A247" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B247" s="0" t="s">
         <v>1110</v>
       </c>
@@ -12608,6 +12698,9 @@
       </c>
     </row>
     <row r="248" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A248" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B248" s="0" t="s">
         <v>1114</v>
       </c>
@@ -12625,6 +12718,9 @@
       </c>
     </row>
     <row r="249" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A249" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B249" s="0" t="s">
         <v>1116</v>
       </c>
@@ -12642,6 +12738,9 @@
       </c>
     </row>
     <row r="250" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A250" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B250" s="0" t="s">
         <v>1119</v>
       </c>
@@ -12662,6 +12761,9 @@
       </c>
     </row>
     <row r="251" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A251" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B251" s="0" t="s">
         <v>1123</v>
       </c>
@@ -12682,6 +12784,9 @@
       </c>
     </row>
     <row r="252" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A252" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B252" s="0" t="s">
         <v>1128</v>
       </c>
@@ -12699,6 +12804,9 @@
       </c>
     </row>
     <row r="253" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A253" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B253" s="0" t="s">
         <v>1132</v>
       </c>
@@ -12719,6 +12827,9 @@
       </c>
     </row>
     <row r="254" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A254" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B254" s="0" t="s">
         <v>1136</v>
       </c>
@@ -12736,6 +12847,9 @@
       </c>
     </row>
     <row r="255" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A255" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B255" s="0" t="s">
         <v>1140</v>
       </c>
@@ -12753,6 +12867,9 @@
       </c>
     </row>
     <row r="256" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A256" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B256" s="0" t="s">
         <v>1144</v>
       </c>
@@ -12770,6 +12887,9 @@
       </c>
     </row>
     <row r="257" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A257" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B257" s="0" t="s">
         <v>1148</v>
       </c>
@@ -12787,6 +12907,9 @@
       </c>
     </row>
     <row r="258" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A258" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B258" s="0" t="s">
         <v>1151</v>
       </c>
@@ -12804,6 +12927,9 @@
       </c>
     </row>
     <row r="259" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A259" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B259" s="0" t="s">
         <v>1155</v>
       </c>
@@ -12821,6 +12947,9 @@
       </c>
     </row>
     <row r="260" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A260" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B260" s="0" t="s">
         <v>1159</v>
       </c>
@@ -12838,6 +12967,9 @@
       </c>
     </row>
     <row r="261" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A261" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B261" s="0" t="s">
         <v>1162</v>
       </c>
@@ -12855,6 +12987,9 @@
       </c>
     </row>
     <row r="262" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A262" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B262" s="0" t="s">
         <v>1166</v>
       </c>
@@ -12873,6 +13008,9 @@
       <c r="H262" s="44"/>
     </row>
     <row r="263" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A263" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B263" s="0" t="s">
         <v>1170</v>
       </c>
@@ -12893,6 +13031,9 @@
       </c>
     </row>
     <row r="264" s="16" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A264" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B264" s="16" t="s">
         <v>1174</v>
       </c>
@@ -12900,6 +13041,9 @@
       <c r="H264" s="31"/>
     </row>
     <row r="265" s="33" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A265" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B265" s="33" t="s">
         <v>1175</v>
       </c>
@@ -12921,6 +13065,9 @@
       </c>
     </row>
     <row r="266" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A266" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B266" s="0" t="s">
         <v>1178</v>
       </c>
@@ -12938,6 +13085,9 @@
       </c>
     </row>
     <row r="267" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A267" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B267" s="0" t="s">
         <v>1182</v>
       </c>
@@ -12955,6 +13105,9 @@
       </c>
     </row>
     <row r="268" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A268" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B268" s="0" t="s">
         <v>1185</v>
       </c>
@@ -12972,6 +13125,9 @@
       </c>
     </row>
     <row r="269" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A269" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B269" s="0" t="s">
         <v>1189</v>
       </c>
@@ -12989,6 +13145,9 @@
       </c>
     </row>
     <row r="270" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A270" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B270" s="0" t="s">
         <v>1193</v>
       </c>
@@ -13006,6 +13165,9 @@
       </c>
     </row>
     <row r="271" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A271" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B271" s="0" t="s">
         <v>1197</v>
       </c>
@@ -13023,6 +13185,9 @@
       </c>
     </row>
     <row r="272" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A272" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B272" s="0" t="s">
         <v>1201</v>
       </c>
@@ -13040,6 +13205,9 @@
       </c>
     </row>
     <row r="273" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A273" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B273" s="0" t="s">
         <v>1206</v>
       </c>
@@ -13060,6 +13228,9 @@
       </c>
     </row>
     <row r="274" s="33" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A274" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B274" s="45" t="s">
         <v>1210</v>
       </c>
@@ -13081,6 +13252,9 @@
       </c>
     </row>
     <row r="275" s="16" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A275" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B275" s="16" t="s">
         <v>1213</v>
       </c>
@@ -13088,6 +13262,9 @@
       <c r="H275" s="31"/>
     </row>
     <row r="276" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A276" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B276" s="20" t="s">
         <v>1214</v>
       </c>
@@ -13102,6 +13279,9 @@
       </c>
     </row>
     <row r="277" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A277" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B277" s="20" t="s">
         <v>1217</v>
       </c>
@@ -13122,6 +13302,9 @@
       </c>
     </row>
     <row r="278" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A278" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B278" s="0" t="s">
         <v>1222</v>
       </c>
@@ -13142,6 +13325,9 @@
       </c>
     </row>
     <row r="279" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A279" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B279" s="0" t="s">
         <v>1227</v>
       </c>
@@ -13162,6 +13348,9 @@
       </c>
     </row>
     <row r="280" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A280" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B280" s="0" t="s">
         <v>1232</v>
       </c>
@@ -13182,6 +13371,9 @@
       </c>
     </row>
     <row r="281" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A281" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B281" s="0" t="s">
         <v>1237</v>
       </c>
@@ -13199,6 +13391,9 @@
       </c>
     </row>
     <row r="282" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A282" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B282" s="0" t="s">
         <v>1239</v>
       </c>
@@ -13216,6 +13411,9 @@
       </c>
     </row>
     <row r="283" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A283" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B283" s="0" t="s">
         <v>1242</v>
       </c>
@@ -13233,6 +13431,9 @@
       </c>
     </row>
     <row r="284" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A284" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B284" s="0" t="s">
         <v>1246</v>
       </c>
@@ -13250,6 +13451,9 @@
       </c>
     </row>
     <row r="285" s="16" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A285" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B285" s="16" t="s">
         <v>1250</v>
       </c>
@@ -13257,6 +13461,9 @@
       <c r="H285" s="31"/>
     </row>
     <row r="286" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A286" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B286" s="0" t="s">
         <v>1251</v>
       </c>
@@ -13277,6 +13484,9 @@
       </c>
     </row>
     <row r="287" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A287" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B287" s="0" t="s">
         <v>1256</v>
       </c>
@@ -13297,6 +13507,9 @@
       </c>
     </row>
     <row r="288" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A288" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B288" s="0" t="s">
         <v>1261</v>
       </c>
@@ -13317,6 +13530,9 @@
       </c>
     </row>
     <row r="289" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A289" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B289" s="0" t="s">
         <v>1266</v>
       </c>
@@ -13337,6 +13553,9 @@
       </c>
     </row>
     <row r="290" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A290" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B290" s="0" t="s">
         <v>1271</v>
       </c>
@@ -13357,6 +13576,9 @@
       </c>
     </row>
     <row r="291" s="16" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A291" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B291" s="16" t="s">
         <v>1276</v>
       </c>
@@ -13364,6 +13586,9 @@
       <c r="H291" s="31"/>
     </row>
     <row r="292" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A292" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B292" s="0" t="s">
         <v>1277</v>
       </c>
@@ -13384,6 +13609,9 @@
       </c>
     </row>
     <row r="293" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A293" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B293" s="0" t="s">
         <v>1282</v>
       </c>
@@ -13404,6 +13632,9 @@
       </c>
     </row>
     <row r="294" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A294" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B294" s="0" t="s">
         <v>1287</v>
       </c>
@@ -13421,6 +13652,9 @@
       </c>
     </row>
     <row r="295" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A295" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B295" s="0" t="s">
         <v>1290</v>
       </c>
@@ -13438,6 +13672,9 @@
       </c>
     </row>
     <row r="296" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A296" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B296" s="0" t="s">
         <v>1294</v>
       </c>
@@ -13455,6 +13692,9 @@
       </c>
     </row>
     <row r="297" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A297" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B297" s="0" t="s">
         <v>1297</v>
       </c>
@@ -13472,6 +13712,9 @@
       </c>
     </row>
     <row r="298" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A298" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B298" s="0" t="s">
         <v>1301</v>
       </c>
@@ -13490,6 +13733,9 @@
       <c r="H298" s="46"/>
     </row>
     <row r="299" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A299" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B299" s="0" t="s">
         <v>1305</v>
       </c>
@@ -13507,6 +13753,9 @@
       </c>
     </row>
     <row r="300" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A300" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B300" s="0" t="s">
         <v>1309</v>
       </c>
@@ -13524,6 +13773,9 @@
       </c>
     </row>
     <row r="301" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A301" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B301" s="0" t="s">
         <v>1313</v>
       </c>
@@ -13541,6 +13793,9 @@
       </c>
     </row>
     <row r="302" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A302" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B302" s="0" t="s">
         <v>1317</v>
       </c>
@@ -13558,6 +13813,9 @@
       </c>
     </row>
     <row r="303" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A303" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B303" s="0" t="s">
         <v>1321</v>
       </c>
@@ -13575,6 +13833,9 @@
       </c>
     </row>
     <row r="304" s="16" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A304" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B304" s="16" t="s">
         <v>1324</v>
       </c>
@@ -13582,6 +13843,9 @@
       <c r="H304" s="31"/>
     </row>
     <row r="305" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A305" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B305" s="0" t="s">
         <v>1325</v>
       </c>
@@ -13599,6 +13863,9 @@
       </c>
     </row>
     <row r="306" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A306" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B306" s="0" t="s">
         <v>1329</v>
       </c>
@@ -13616,6 +13883,9 @@
       </c>
     </row>
     <row r="307" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A307" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B307" s="0" t="s">
         <v>1333</v>
       </c>
@@ -13633,6 +13903,9 @@
       </c>
     </row>
     <row r="308" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A308" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B308" s="0" t="s">
         <v>1338</v>
       </c>
@@ -13650,6 +13923,9 @@
       </c>
     </row>
     <row r="309" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A309" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B309" s="0" t="s">
         <v>1341</v>
       </c>
@@ -13670,6 +13946,9 @@
       </c>
     </row>
     <row r="310" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A310" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B310" s="0" t="s">
         <v>1346</v>
       </c>
@@ -13690,6 +13969,9 @@
       </c>
     </row>
     <row r="311" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A311" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B311" s="0" t="s">
         <v>1351</v>
       </c>
@@ -13710,6 +13992,9 @@
       </c>
     </row>
     <row r="312" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A312" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B312" s="0" t="s">
         <v>1356</v>
       </c>
@@ -13727,6 +14012,9 @@
       </c>
     </row>
     <row r="313" s="33" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A313" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B313" s="33" t="s">
         <v>1360</v>
       </c>
@@ -13745,6 +14033,9 @@
       <c r="H313" s="37"/>
     </row>
     <row r="314" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A314" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B314" s="0" t="s">
         <v>1363</v>
       </c>
@@ -13762,6 +14053,9 @@
       </c>
     </row>
     <row r="315" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A315" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B315" s="0" t="s">
         <v>1366</v>
       </c>
@@ -13779,6 +14073,9 @@
       </c>
     </row>
     <row r="316" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A316" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B316" s="0" t="s">
         <v>1370</v>
       </c>
@@ -13796,6 +14093,9 @@
       </c>
     </row>
     <row r="317" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A317" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B317" s="0" t="s">
         <v>1374</v>
       </c>
@@ -13813,6 +14113,9 @@
       </c>
     </row>
     <row r="318" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A318" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B318" s="0" t="s">
         <v>1378</v>
       </c>
@@ -13830,6 +14133,9 @@
       </c>
     </row>
     <row r="319" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A319" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B319" s="0" t="s">
         <v>1382</v>
       </c>
@@ -13853,6 +14159,9 @@
       </c>
     </row>
     <row r="320" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A320" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B320" s="0" t="s">
         <v>1389</v>
       </c>
@@ -13876,6 +14185,9 @@
       </c>
     </row>
     <row r="321" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A321" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B321" s="0" t="s">
         <v>52</v>
       </c>
@@ -13899,6 +14211,9 @@
       </c>
     </row>
     <row r="322" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A322" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B322" s="0" t="s">
         <v>1400</v>
       </c>
@@ -13916,6 +14231,9 @@
       </c>
     </row>
     <row r="323" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A323" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B323" s="0" t="s">
         <v>1403</v>
       </c>
@@ -13933,6 +14251,9 @@
       </c>
     </row>
     <row r="324" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A324" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B324" s="0" t="s">
         <v>1405</v>
       </c>
@@ -13953,6 +14274,9 @@
       </c>
     </row>
     <row r="325" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A325" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B325" s="0" t="s">
         <v>1410</v>
       </c>
@@ -13973,6 +14297,9 @@
       </c>
     </row>
     <row r="326" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A326" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B326" s="0" t="s">
         <v>1416</v>
       </c>
@@ -13990,6 +14317,9 @@
       </c>
     </row>
     <row r="327" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A327" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B327" s="0" t="s">
         <v>1420</v>
       </c>
@@ -14007,6 +14337,9 @@
       </c>
     </row>
     <row r="328" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A328" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B328" s="0" t="s">
         <v>1424</v>
       </c>
@@ -14024,6 +14357,9 @@
       </c>
     </row>
     <row r="329" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A329" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B329" s="0" t="s">
         <v>237</v>
       </c>
@@ -14044,6 +14380,9 @@
       </c>
     </row>
     <row r="330" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A330" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B330" s="0" t="s">
         <v>1429</v>
       </c>
@@ -14064,6 +14403,9 @@
       </c>
     </row>
     <row r="331" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A331" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B331" s="0" t="s">
         <v>1431</v>
       </c>
@@ -14084,6 +14426,9 @@
       </c>
     </row>
     <row r="332" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A332" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B332" s="0" t="s">
         <v>1435</v>
       </c>
@@ -14113,6 +14458,9 @@
       </c>
     </row>
     <row r="333" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A333" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B333" s="0" t="s">
         <v>1442</v>
       </c>
@@ -14136,6 +14484,9 @@
       </c>
     </row>
     <row r="334" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A334" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B334" s="0" t="s">
         <v>1447</v>
       </c>
@@ -14153,6 +14504,9 @@
       </c>
     </row>
     <row r="335" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A335" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B335" s="0" t="s">
         <v>1450</v>
       </c>
@@ -14173,6 +14527,9 @@
       </c>
     </row>
     <row r="336" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A336" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B336" s="0" t="s">
         <v>1454</v>
       </c>
@@ -14193,6 +14550,9 @@
       </c>
     </row>
     <row r="337" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A337" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B337" s="0" t="s">
         <v>1378</v>
       </c>
@@ -14213,6 +14573,9 @@
       </c>
     </row>
     <row r="338" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A338" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B338" s="0" t="s">
         <v>1462</v>
       </c>
@@ -14233,6 +14596,9 @@
       </c>
     </row>
     <row r="339" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A339" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B339" s="0" t="s">
         <v>1467</v>
       </c>
@@ -14253,6 +14619,9 @@
       </c>
     </row>
     <row r="340" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A340" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B340" s="0" t="s">
         <v>1471</v>
       </c>
@@ -14270,6 +14639,9 @@
       </c>
     </row>
     <row r="341" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A341" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B341" s="0" t="s">
         <v>1474</v>
       </c>
@@ -14290,6 +14662,9 @@
       </c>
     </row>
     <row r="342" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A342" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B342" s="0" t="s">
         <v>1479</v>
       </c>
@@ -14307,6 +14682,9 @@
       </c>
     </row>
     <row r="343" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A343" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B343" s="0" t="s">
         <v>1481</v>
       </c>
@@ -14327,6 +14705,9 @@
       </c>
     </row>
     <row r="344" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A344" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B344" s="0" t="s">
         <v>1486</v>
       </c>
@@ -14341,6 +14722,9 @@
       </c>
     </row>
     <row r="345" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A345" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B345" s="0" t="s">
         <v>1490</v>
       </c>
@@ -14358,6 +14742,9 @@
       </c>
     </row>
     <row r="346" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A346" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B346" s="0" t="s">
         <v>1494</v>
       </c>
@@ -14375,6 +14762,9 @@
       </c>
     </row>
     <row r="347" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A347" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B347" s="0" t="s">
         <v>1498</v>
       </c>
@@ -14392,6 +14782,9 @@
       </c>
     </row>
     <row r="348" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A348" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B348" s="0" t="s">
         <v>1501</v>
       </c>
@@ -14409,6 +14802,9 @@
       </c>
     </row>
     <row r="349" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A349" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B349" s="0" t="s">
         <v>1504</v>
       </c>
@@ -14426,6 +14822,9 @@
       </c>
     </row>
     <row r="350" s="33" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A350" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B350" s="33" t="s">
         <v>1507</v>
       </c>
@@ -14447,6 +14846,9 @@
       </c>
     </row>
     <row r="351" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A351" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="B351" s="0" t="s">
         <v>1511</v>
       </c>
@@ -14467,6 +14869,9 @@
       </c>
     </row>
     <row r="352" s="16" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A352" s="16" t="s">
+        <v>45</v>
+      </c>
       <c r="B352" s="16" t="s">
         <v>1515</v>
       </c>
@@ -14474,6 +14879,9 @@
       <c r="H352" s="31"/>
     </row>
     <row r="353" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A353" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B353" s="0" t="s">
         <v>1516</v>
       </c>
@@ -14494,6 +14902,9 @@
       </c>
     </row>
     <row r="354" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A354" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B354" s="0" t="s">
         <v>1521</v>
       </c>
@@ -14514,6 +14925,9 @@
       </c>
     </row>
     <row r="355" s="16" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A355" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B355" s="16" t="s">
         <v>1525</v>
       </c>
@@ -14521,6 +14935,9 @@
       <c r="H355" s="31"/>
     </row>
     <row r="356" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A356" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B356" s="20" t="s">
         <v>1526</v>
       </c>
@@ -14541,6 +14958,9 @@
       </c>
     </row>
     <row r="357" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A357" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B357" s="0" t="s">
         <v>1531</v>
       </c>
@@ -14555,6 +14975,9 @@
       </c>
     </row>
     <row r="358" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A358" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B358" s="0" t="s">
         <v>1534</v>
       </c>
@@ -14575,6 +14998,9 @@
       </c>
     </row>
     <row r="359" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A359" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B359" s="0" t="s">
         <v>1538</v>
       </c>
@@ -14595,6 +15021,9 @@
       </c>
     </row>
     <row r="360" s="16" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A360" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B360" s="16" t="s">
         <v>1543</v>
       </c>
@@ -14602,6 +15031,9 @@
       <c r="H360" s="31"/>
     </row>
     <row r="361" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A361" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B361" s="0" t="s">
         <v>1544</v>
       </c>
@@ -14622,6 +15054,9 @@
       </c>
     </row>
     <row r="362" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A362" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B362" s="0" t="s">
         <v>1075</v>
       </c>
@@ -14639,6 +15074,9 @@
       </c>
     </row>
     <row r="363" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A363" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B363" s="0" t="s">
         <v>1550</v>
       </c>
@@ -14656,6 +15094,9 @@
       </c>
     </row>
     <row r="364" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A364" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B364" s="0" t="s">
         <v>1554</v>
       </c>
@@ -14673,6 +15114,9 @@
       </c>
     </row>
     <row r="365" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A365" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B365" s="0" t="s">
         <v>1558</v>
       </c>
@@ -14693,6 +15137,9 @@
       </c>
     </row>
     <row r="366" s="34" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A366" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B366" s="34" t="s">
         <v>1563</v>
       </c>
@@ -14711,6 +15158,9 @@
       <c r="H366" s="35"/>
     </row>
     <row r="367" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A367" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="E367" s="0" t="s">
         <v>1566</v>
       </c>
@@ -14719,6 +15169,9 @@
       </c>
     </row>
     <row r="368" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A368" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="E368" s="0" t="s">
         <v>1568</v>
       </c>
@@ -14727,6 +15180,9 @@
       </c>
     </row>
     <row r="369" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A369" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="E369" s="0" t="s">
         <v>1570</v>
       </c>
@@ -14735,12 +15191,18 @@
       </c>
     </row>
     <row r="370" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A370" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="E370" s="0" t="s">
         <v>1572</v>
       </c>
       <c r="G370" s="10"/>
     </row>
     <row r="371" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A371" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="E371" s="0" t="s">
         <v>1573</v>
       </c>
@@ -14749,6 +15211,9 @@
       </c>
     </row>
     <row r="372" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A372" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="E372" s="0" t="s">
         <v>1575</v>
       </c>
@@ -14757,6 +15222,9 @@
       </c>
     </row>
     <row r="373" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A373" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="E373" s="0" t="s">
         <v>1577</v>
       </c>
@@ -14765,6 +15233,9 @@
       </c>
     </row>
     <row r="374" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A374" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="E374" s="0" t="s">
         <v>1579</v>
       </c>
@@ -14773,6 +15244,9 @@
       </c>
     </row>
     <row r="375" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A375" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="E375" s="0" t="s">
         <v>1581</v>
       </c>
@@ -14781,12 +15255,18 @@
       </c>
     </row>
     <row r="376" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A376" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="E376" s="0" t="s">
         <v>1583</v>
       </c>
       <c r="G376" s="10"/>
     </row>
     <row r="377" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A377" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="E377" s="0" t="s">
         <v>1584</v>
       </c>
@@ -14795,6 +15275,9 @@
       </c>
     </row>
     <row r="378" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A378" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="E378" s="0" t="s">
         <v>1586</v>
       </c>
@@ -14803,6 +15286,9 @@
       </c>
     </row>
     <row r="379" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A379" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="E379" s="0" t="s">
         <v>1588</v>
       </c>
@@ -14811,6 +15297,9 @@
       </c>
     </row>
     <row r="380" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A380" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="E380" s="0" t="s">
         <v>1590</v>
       </c>
@@ -14819,6 +15308,9 @@
       </c>
     </row>
     <row r="381" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A381" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="E381" s="0" t="s">
         <v>1592</v>
       </c>
@@ -14827,12 +15319,18 @@
       </c>
     </row>
     <row r="382" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A382" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="E382" s="0" t="s">
         <v>1594</v>
       </c>
       <c r="G382" s="10"/>
     </row>
     <row r="383" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A383" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="E383" s="0" t="s">
         <v>1595</v>
       </c>
@@ -14841,21 +15339,33 @@
       </c>
     </row>
     <row r="384" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A384" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="E384" s="0" t="s">
         <v>1597</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A385" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="E385" s="0" t="s">
         <v>1598</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A386" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="E386" s="0" t="s">
         <v>1599</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A387" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B387" s="0" t="s">
         <v>602</v>
       </c>
@@ -14876,6 +15386,9 @@
       </c>
     </row>
     <row r="388" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A388" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B388" s="0" t="s">
         <v>1604</v>
       </c>
@@ -14893,6 +15406,9 @@
       </c>
     </row>
     <row r="389" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A389" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B389" s="0" t="s">
         <v>1608</v>
       </c>
@@ -14913,6 +15429,9 @@
       </c>
     </row>
     <row r="390" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A390" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B390" s="0" t="s">
         <v>1612</v>
       </c>
@@ -14930,6 +15449,9 @@
       </c>
     </row>
     <row r="391" s="16" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A391" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B391" s="16" t="s">
         <v>1616</v>
       </c>
@@ -14937,6 +15459,9 @@
       <c r="H391" s="31"/>
     </row>
     <row r="392" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A392" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B392" s="0" t="s">
         <v>1617</v>
       </c>
@@ -14954,6 +15479,9 @@
       </c>
     </row>
     <row r="393" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A393" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B393" s="0" t="s">
         <v>1621</v>
       </c>
@@ -14968,6 +15496,9 @@
       </c>
     </row>
     <row r="394" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A394" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B394" s="0" t="s">
         <v>1625</v>
       </c>
@@ -14985,6 +15516,9 @@
       </c>
     </row>
     <row r="395" s="7" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A395" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B395" s="7" t="s">
         <v>1629</v>
       </c>
@@ -15003,6 +15537,9 @@
       <c r="H395" s="8"/>
     </row>
     <row r="396" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A396" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B396" s="0" t="s">
         <v>1633</v>
       </c>
@@ -15023,6 +15560,9 @@
       </c>
     </row>
     <row r="397" s="11" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A397" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B397" s="11" t="s">
         <v>1638</v>
       </c>
@@ -15041,6 +15581,9 @@
       <c r="H397" s="12"/>
     </row>
     <row r="398" s="21" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A398" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B398" s="21" t="s">
         <v>1642</v>
       </c>
@@ -15059,6 +15602,9 @@
       <c r="H398" s="22"/>
     </row>
     <row r="399" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A399" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B399" s="0" t="s">
         <v>1645</v>
       </c>
@@ -15079,6 +15625,9 @@
       </c>
     </row>
     <row r="400" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A400" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B400" s="0" t="s">
         <v>1650</v>
       </c>
@@ -15099,6 +15648,9 @@
       </c>
     </row>
     <row r="401" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A401" s="0" t="s">
+        <v>45</v>
+      </c>
       <c r="B401" s="0" t="s">
         <v>1655</v>
       </c>
@@ -15176,7 +15728,7 @@
   <dimension ref="A1:H157"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A103" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I35" activeCellId="1" sqref="A207:A217 I35"/>
+      <selection pane="topLeft" activeCell="I35" activeCellId="1" sqref="A367:A386 I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18716,7 +19268,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A207:A217 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A367:A386 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>